<commit_message>
99% result (change summ_str)
</commit_message>
<xml_diff>
--- a/xlsx/test.xlsx
+++ b/xlsx/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Python\BUP_bot\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C89B9-84B3-4F5A-886E-209E66E81631}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BC9B70-4C49-4A9C-A0C2-BA90BEDEACCB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="32760" yWindow="32760" windowWidth="18780" windowHeight="10920" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,15 +162,6 @@
     <t>Пауч для ламинирования 80 мкм, 75х52 мм, уп. 100 шт.</t>
   </si>
   <si>
-    <t>(0176) 77-19-72   Приемная директора</t>
-  </si>
-  <si>
-    <t>Сто девяносто два  рубля 00 копеек.</t>
-  </si>
-  <si>
-    <t>Тридцать два рубля 00 копеек.</t>
-  </si>
-  <si>
     <t>2. Предоплата, в размере 100% стоимости товара, производится Покупателем на счёт Поставщика в течение 3-х банковских дней по факту поставки.</t>
   </si>
   <si>
@@ -198,11 +189,19 @@
     <t>Счет-фактура №</t>
   </si>
   <si>
-    <t xml:space="preserve"> ОАО "Гродненская табачная фабрика "Неман"
-</t>
-  </si>
-  <si>
     <t>3. Срок поставки: не позднее 5-и рабочих дней с момента подписания счет-фактуры - протокола согласования договорной цены. (в наличии).</t>
+  </si>
+  <si>
+    <t>ОАО "пример"</t>
+  </si>
+  <si>
+    <t>бла-бла-бла</t>
+  </si>
+  <si>
+    <t>сорок рублей ноль копеек</t>
+  </si>
+  <si>
+    <t>шесть рублей ноль копеек</t>
   </si>
 </sst>
 </file>
@@ -578,9 +577,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -607,48 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,74 +1157,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
       <c r="D1" s="18"/>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67">
-        <v>15</v>
-      </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="A2" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50">
+        <v>20</v>
+      </c>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64">
-        <v>43969</v>
-      </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
+      <c r="A4" s="46">
+        <v>43970</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:10" s="24" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="25"/>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="1:10" s="24" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="1:10" s="24" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
@@ -1239,70 +1238,70 @@
     <row r="8" spans="1:10" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:10" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
+      <c r="C9" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
     </row>
     <row r="10" spans="1:10" s="24" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
+      <c r="C10" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
     </row>
     <row r="11" spans="1:10" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="47"/>
+      <c r="C11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" s="7" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="59"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="20" t="s">
         <v>6</v>
       </c>
@@ -1329,33 +1328,33 @@
       <c r="A14" s="36">
         <v>1</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="61"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="36">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="E14" s="36" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="38">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G14" s="38">
         <f>F14*D14</f>
-        <v>120</v>
+        <v>10.5</v>
       </c>
       <c r="H14" s="39">
         <v>20</v>
       </c>
       <c r="I14" s="38">
         <f>G14*0.2</f>
-        <v>24</v>
+        <v>2.1</v>
       </c>
       <c r="J14" s="38">
         <f>I14+G14</f>
-        <v>144</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1" ht="66.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1374,33 +1373,33 @@
       <c r="A16" s="36">
         <v>2</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>35</v>
       </c>
       <c r="F16" s="38">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G16" s="38">
         <f>F16*D16</f>
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H16" s="39">
         <v>20</v>
       </c>
       <c r="I16" s="38">
         <f>G16*0.2</f>
-        <v>8</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="J16" s="38">
         <f>I16+G16</f>
-        <v>48</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1421,7 +1420,7 @@
       </c>
       <c r="J18" s="28">
         <f>SUM(J14:J17)</f>
-        <v>192</v>
+        <v>40.200000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -1439,38 +1438,38 @@
       </c>
       <c r="J20" s="30">
         <f>J18/6</f>
-        <v>32</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
+      <c r="C21" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
     </row>
     <row r="22" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
+      <c r="C22" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
     </row>
     <row r="23" spans="1:11" ht="0.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1489,38 +1488,38 @@
       <c r="K24" s="31"/>
     </row>
     <row r="25" spans="1:11" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
+      <c r="A25" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
       <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" s="24" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
+      <c r="A26" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
       <c r="K26" s="31"/>
     </row>
     <row r="27" spans="1:11" s="24" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="31"/>
@@ -1534,23 +1533,23 @@
       <c r="K27" s="31"/>
     </row>
     <row r="28" spans="1:11" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
       <c r="K28" s="31"/>
     </row>
     <row r="29" spans="1:11" s="24" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="31"/>
@@ -1564,62 +1563,62 @@
       <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
+      <c r="A30" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
     </row>
     <row r="31" spans="1:11" ht="33.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
     </row>
     <row r="32" spans="1:11" ht="34.15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50" t="s">
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="51"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="65"/>
     </row>
     <row r="33" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
     </row>
     <row r="34" spans="2:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
@@ -1628,10 +1627,10 @@
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="17"/>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="46"/>
+      <c r="G34" s="60"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
@@ -1680,13 +1679,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="B33:J33"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="C22:J22"/>
     <mergeCell ref="C5:J6"/>
@@ -1696,15 +1697,13 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>